<commit_message>
Update initial time to 2021
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/IT/Initial Time.xlsx
+++ b/InputData/plcy-schd/IT/Initial Time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\us-eps\InputData\plcy-schd\IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\plcy-schd\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DA93EC-B5DF-4DB0-97B6-F21DB44D41D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC6B9E6-8492-47B5-AB74-054F3998C509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="840" windowWidth="15615" windowHeight="15645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -127,13 +127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -502,7 +501,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -580,7 +579,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -596,7 +595,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>